<commit_message>
Added in code to plot outliers
</commit_message>
<xml_diff>
--- a/191027_Deuterium_Transfer_Peak_Areas.xlsx
+++ b/191027_Deuterium_Transfer_Peak_Areas.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\Parker_research\GCMS_Stuff\191027\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/TomNaragon/Desktop/Parker_Research/DCHC_transfer_Experiment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37C4193-A7E5-48D9-81F2-E898423DC34F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-230" yWindow="1560" windowWidth="38360" windowHeight="19310" xr2:uid="{0C4FD04D-EEC1-4A1F-94F8-64C84F3860BB}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16860" windowHeight="17540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="26">
   <si>
     <t>Species</t>
   </si>
@@ -90,9 +95,6 @@
     <t>#Type refers to deuterium labelled ants (L) vs unlabelled ants (U)</t>
   </si>
   <si>
-    <t>#Outlier: Beetle or ant crushed/Beetle or ant escaped from well/Ant not coated in any CHCs (Y), Beetle chomped (B), ant chomped (A), normal run (N)</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -107,15 +109,28 @@
   <si>
     <t>N</t>
   </si>
+  <si>
+    <t>#Outlier: Beetle or ant crushed/Beetle or ant escaped from well/Ant not coated in any CHCs (Y); Beetle chomped (B); ant chomped (A); ant injured from the beginning(AI); beetle injured/dessicates early(BI); normal run (N)</t>
+  </si>
+  <si>
+    <t>AI</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -141,8 +156,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,31 +472,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9318726-D8BA-4845-AE33-2EE2376C2E04}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -518,13 +534,13 @@
         <v>11</v>
       </c>
       <c r="M4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N4" t="s">
         <v>20</v>
       </c>
-      <c r="N4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -565,10 +581,10 @@
         <v>12</v>
       </c>
       <c r="N5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -609,10 +625,10 @@
         <v>12</v>
       </c>
       <c r="N6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -653,10 +669,10 @@
         <v>12</v>
       </c>
       <c r="N7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -697,10 +713,10 @@
         <v>12</v>
       </c>
       <c r="N8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -741,10 +757,10 @@
         <v>12</v>
       </c>
       <c r="N9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -785,10 +801,10 @@
         <v>12</v>
       </c>
       <c r="N10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -826,13 +842,13 @@
         <v>0.85</v>
       </c>
       <c r="M11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -870,13 +886,13 @@
         <v>1.75</v>
       </c>
       <c r="M12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -914,13 +930,13 @@
         <v>1.07</v>
       </c>
       <c r="M13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -958,13 +974,13 @@
         <v>0.81</v>
       </c>
       <c r="M14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1002,13 +1018,13 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="M15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1046,13 +1062,13 @@
         <v>1.97</v>
       </c>
       <c r="M16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1090,13 +1106,13 @@
         <v>0.82</v>
       </c>
       <c r="M17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -1134,13 +1150,13 @@
         <v>1.42</v>
       </c>
       <c r="M18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -1178,13 +1194,13 @@
         <v>0.86</v>
       </c>
       <c r="M19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N19" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -1222,13 +1238,13 @@
         <v>0.81</v>
       </c>
       <c r="M20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -1266,13 +1282,13 @@
         <v>1.44</v>
       </c>
       <c r="M21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -1310,13 +1326,13 @@
         <v>2.2599999999999998</v>
       </c>
       <c r="M22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -1357,10 +1373,10 @@
         <v>12</v>
       </c>
       <c r="N23" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>12</v>
       </c>
@@ -1401,10 +1417,10 @@
         <v>12</v>
       </c>
       <c r="N24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -1445,10 +1461,10 @@
         <v>12</v>
       </c>
       <c r="N25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -1489,10 +1505,10 @@
         <v>12</v>
       </c>
       <c r="N26" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -1533,10 +1549,10 @@
         <v>12</v>
       </c>
       <c r="N27" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -1577,10 +1593,10 @@
         <v>12</v>
       </c>
       <c r="N28" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>12</v>
       </c>
@@ -1618,13 +1634,13 @@
         <v>0.87</v>
       </c>
       <c r="M29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N29" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -1662,13 +1678,13 @@
         <v>2.09</v>
       </c>
       <c r="M30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N30" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>12</v>
       </c>
@@ -1706,13 +1722,13 @@
         <v>0.91</v>
       </c>
       <c r="M31" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N31" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>17</v>
       </c>
@@ -1750,13 +1766,13 @@
         <v>0.81</v>
       </c>
       <c r="M32" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N32" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>17</v>
       </c>
@@ -1794,13 +1810,13 @@
         <v>1.37</v>
       </c>
       <c r="M33" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N33" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>17</v>
       </c>
@@ -1838,13 +1854,13 @@
         <v>2.25</v>
       </c>
       <c r="M34" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N34" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -1885,10 +1901,10 @@
         <v>12</v>
       </c>
       <c r="N35" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -1929,10 +1945,10 @@
         <v>12</v>
       </c>
       <c r="N36" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>12</v>
       </c>
@@ -1973,10 +1989,10 @@
         <v>12</v>
       </c>
       <c r="N37" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>17</v>
       </c>
@@ -2017,10 +2033,10 @@
         <v>12</v>
       </c>
       <c r="N38" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>17</v>
       </c>
@@ -2061,10 +2077,10 @@
         <v>12</v>
       </c>
       <c r="N39" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>17</v>
       </c>
@@ -2105,10 +2121,10 @@
         <v>12</v>
       </c>
       <c r="N40" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -2149,10 +2165,10 @@
         <v>12</v>
       </c>
       <c r="N41" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -2193,10 +2209,10 @@
         <v>12</v>
       </c>
       <c r="N42" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -2237,10 +2253,10 @@
         <v>12</v>
       </c>
       <c r="N43" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>17</v>
       </c>
@@ -2281,10 +2297,10 @@
         <v>12</v>
       </c>
       <c r="N44" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>17</v>
       </c>
@@ -2325,10 +2341,10 @@
         <v>12</v>
       </c>
       <c r="N45" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>17</v>
       </c>
@@ -2369,10 +2385,10 @@
         <v>12</v>
       </c>
       <c r="N46" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>12</v>
       </c>
@@ -2410,13 +2426,13 @@
         <v>0.83</v>
       </c>
       <c r="M47" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N47" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>12</v>
       </c>
@@ -2454,13 +2470,13 @@
         <v>1.69</v>
       </c>
       <c r="M48" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N48" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>12</v>
       </c>
@@ -2498,13 +2514,13 @@
         <v>1.06</v>
       </c>
       <c r="M49" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N49" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>17</v>
       </c>
@@ -2542,13 +2558,13 @@
         <v>0.79</v>
       </c>
       <c r="M50" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N50" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>17</v>
       </c>
@@ -2586,13 +2602,13 @@
         <v>1.2</v>
       </c>
       <c r="M51" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N51" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>17</v>
       </c>
@@ -2630,10 +2646,10 @@
         <v>2.2400000000000002</v>
       </c>
       <c r="M52" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N52" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>